<commit_message>
manual curve and PARAMS #6
</commit_message>
<xml_diff>
--- a/other_data/manual_growth_curves.xlsx
+++ b/other_data/manual_growth_curves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/other_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CADC6E-EAEC-054D-97EC-BA0D5BB6198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F287FE57-87BD-0C4F-83C7-981D931B1D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,40 +1990,40 @@
                   <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.47333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.74333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.0666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1.5433333333333332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.0233333333333334</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2.6066666666666669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3.2399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3.76</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>4.541666666666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>5.69</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>6.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2149,40 +2149,40 @@
                   <c:v>0.14333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.17666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.24666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.3666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.5033333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.80666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.4400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.5466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1.9233333333333331</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2.3066666666666666</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2.4616666666666664</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3.206666666666667</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3.5066666666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2308,40 +2308,40 @@
                   <c:v>0.32666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.53333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2.4866666666666668</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3.6199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4.9866666666666672</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>6.7633333333333328</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>8.4066666666666663</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>9.49</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>9.5583333333333318</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>11.433333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>11.450000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2467,40 +2467,40 @@
                   <c:v>0.18333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.24333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.29333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.51333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.79999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1.2233333333333334</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2.0666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2.6199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3.0333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3.3133333333333339</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3.9733333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>4.4366666666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6132,7 +6132,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6422,288 +6422,695 @@
       <c r="A6" s="20">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="19">
+        <v>0.32</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.37</v>
+      </c>
       <c r="E6" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0.18</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0.19</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0.16</v>
       </c>
       <c r="I6" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.17666666666666667</v>
+      </c>
+      <c r="J6" s="21">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.51</v>
+      </c>
+      <c r="L6" s="21">
+        <v>0.54</v>
       </c>
       <c r="M6" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P6" s="21">
+        <v>0.24</v>
       </c>
       <c r="Q6" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.24333333333333332</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>2.5</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="19">
+        <v>0.47</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.46</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.49</v>
+      </c>
       <c r="E7" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.47333333333333333</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0.25</v>
       </c>
       <c r="I7" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24666666666666667</v>
+      </c>
+      <c r="J7" s="21">
+        <v>0.89</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.86</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0.89</v>
       </c>
       <c r="M7" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.88</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="P7" s="21">
+        <v>0.33</v>
       </c>
       <c r="Q7" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.29333333333333339</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="19">
+        <v>0.74</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0.74</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.75</v>
+      </c>
       <c r="E8" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.74333333333333329</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0.35</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="J8" s="21">
+        <v>1.57</v>
+      </c>
+      <c r="K8" s="21">
+        <v>1.46</v>
+      </c>
+      <c r="L8" s="21">
+        <v>1.56</v>
       </c>
       <c r="M8" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.53</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0.47</v>
+      </c>
+      <c r="O8" s="21">
+        <v>0.45</v>
+      </c>
+      <c r="P8" s="21">
+        <v>0.62</v>
       </c>
       <c r="Q8" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.51333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>3.5</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="19">
+        <v>1.17</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1.02</v>
+      </c>
+      <c r="D9" s="19">
+        <v>1.01</v>
+      </c>
       <c r="E9" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.51</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0.46</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0.54</v>
       </c>
       <c r="I9" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5033333333333333</v>
+      </c>
+      <c r="J9" s="21">
+        <v>2.71</v>
+      </c>
+      <c r="K9" s="21">
+        <v>2.35</v>
+      </c>
+      <c r="L9" s="21">
+        <v>2.4</v>
       </c>
       <c r="M9" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.4866666666666668</v>
+      </c>
+      <c r="N9" s="21">
+        <v>0.77</v>
+      </c>
+      <c r="O9" s="21">
+        <v>0.76</v>
+      </c>
+      <c r="P9" s="21">
+        <v>0.87</v>
       </c>
       <c r="Q9" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>4</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19">
+        <v>1.59</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1.55</v>
+      </c>
+      <c r="D10" s="19">
+        <v>1.49</v>
+      </c>
       <c r="E10" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5433333333333332</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.81</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.81</v>
       </c>
       <c r="I10" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.80666666666666664</v>
+      </c>
+      <c r="J10" s="21">
+        <v>3.82</v>
+      </c>
+      <c r="K10" s="21">
+        <v>3.32</v>
+      </c>
+      <c r="L10" s="21">
+        <v>3.72</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.6199999999999997</v>
+      </c>
+      <c r="N10" s="21">
+        <v>1.17</v>
+      </c>
+      <c r="O10" s="21">
+        <v>1.18</v>
+      </c>
+      <c r="P10" s="21">
+        <v>1.32</v>
       </c>
       <c r="Q10" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.2233333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>4.5</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19">
+        <v>2.02</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2.04</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2.0099999999999998</v>
+      </c>
       <c r="E11" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0233333333333334</v>
+      </c>
+      <c r="F11" s="21">
+        <v>1.17</v>
+      </c>
+      <c r="G11" s="21">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H11" s="21">
+        <v>1.99</v>
       </c>
       <c r="I11" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4400000000000002</v>
+      </c>
+      <c r="J11" s="21">
+        <v>5.36</v>
+      </c>
+      <c r="K11" s="21">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="L11" s="21">
+        <v>4.91</v>
       </c>
       <c r="M11" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.9866666666666672</v>
+      </c>
+      <c r="N11" s="21">
+        <v>1.65</v>
+      </c>
+      <c r="O11" s="21">
+        <v>1.64</v>
+      </c>
+      <c r="P11" s="21">
+        <v>1.71</v>
       </c>
       <c r="Q11" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>5</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19">
+        <v>2.61</v>
+      </c>
+      <c r="C12" s="19">
+        <v>2.7</v>
+      </c>
+      <c r="D12" s="19">
+        <v>2.5099999999999998</v>
+      </c>
       <c r="E12" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.6066666666666669</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1.57</v>
+      </c>
+      <c r="G12" s="21">
+        <v>1.49</v>
+      </c>
+      <c r="H12" s="21">
+        <v>1.58</v>
       </c>
       <c r="I12" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5466666666666669</v>
+      </c>
+      <c r="J12" s="21">
+        <v>7.3</v>
+      </c>
+      <c r="K12" s="21">
+        <v>6.27</v>
+      </c>
+      <c r="L12" s="21">
+        <v>6.72</v>
       </c>
       <c r="M12" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.7633333333333328</v>
+      </c>
+      <c r="N12" s="21">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="O12" s="21">
+        <v>2.04</v>
+      </c>
+      <c r="P12" s="21">
+        <v>2.15</v>
       </c>
       <c r="Q12" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.0666666666666664</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>5.5</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="B13" s="19">
+        <v>3.26</v>
+      </c>
+      <c r="C13" s="19">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="19">
+        <v>3.21</v>
+      </c>
       <c r="E13" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.2399999999999998</v>
+      </c>
+      <c r="F13" s="21">
+        <v>1.98</v>
+      </c>
+      <c r="G13" s="21">
+        <v>1.85</v>
+      </c>
+      <c r="H13" s="21">
+        <v>1.94</v>
       </c>
       <c r="I13" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9233333333333331</v>
+      </c>
+      <c r="J13" s="21">
+        <v>8.74</v>
+      </c>
+      <c r="K13" s="21">
+        <v>7.86</v>
+      </c>
+      <c r="L13" s="21">
+        <v>8.6199999999999992</v>
       </c>
       <c r="M13" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.4066666666666663</v>
+      </c>
+      <c r="N13" s="21">
+        <v>2.62</v>
+      </c>
+      <c r="O13" s="21">
+        <v>2.56</v>
+      </c>
+      <c r="P13" s="21">
+        <v>2.68</v>
       </c>
       <c r="Q13" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.6199999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>6</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="B14" s="19">
+        <v>3.78</v>
+      </c>
+      <c r="C14" s="19">
+        <v>3.65</v>
+      </c>
+      <c r="D14" s="19">
+        <v>3.85</v>
+      </c>
       <c r="E14" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.76</v>
+      </c>
+      <c r="F14" s="21">
+        <v>2.27</v>
+      </c>
+      <c r="G14" s="21">
+        <v>2.31</v>
+      </c>
+      <c r="H14" s="21">
+        <v>2.34</v>
       </c>
       <c r="I14" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.3066666666666666</v>
+      </c>
+      <c r="J14" s="21">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="K14" s="21">
+        <v>8.83</v>
+      </c>
+      <c r="L14" s="21">
+        <v>9.68</v>
       </c>
       <c r="M14" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.49</v>
+      </c>
+      <c r="N14" s="21">
+        <v>3.06</v>
+      </c>
+      <c r="O14" s="21">
+        <v>3.02</v>
+      </c>
+      <c r="P14" s="21">
+        <v>3.02</v>
       </c>
       <c r="Q14" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.0333333333333332</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>6.5</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="19">
+        <f>9.36/2</f>
+        <v>4.68</v>
+      </c>
+      <c r="C15" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="D15" s="19">
+        <f>8.89/2</f>
+        <v>4.4450000000000003</v>
+      </c>
       <c r="E15" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.541666666666667</v>
+      </c>
+      <c r="F15">
+        <f>4.97/2</f>
+        <v>2.4849999999999999</v>
+      </c>
+      <c r="G15">
+        <f>4.89/2</f>
+        <v>2.4449999999999998</v>
+      </c>
+      <c r="H15">
+        <f>4.91/2</f>
+        <v>2.4550000000000001</v>
       </c>
       <c r="I15" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.4616666666666664</v>
+      </c>
+      <c r="J15">
+        <f>19.85/2</f>
+        <v>9.9250000000000007</v>
+      </c>
+      <c r="K15">
+        <f>18.37/2</f>
+        <v>9.1850000000000005</v>
+      </c>
+      <c r="L15">
+        <f>19.13/2</f>
+        <v>9.5649999999999995</v>
       </c>
       <c r="M15" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.5583333333333318</v>
+      </c>
+      <c r="N15">
+        <f>6.61/2</f>
+        <v>3.3050000000000002</v>
+      </c>
+      <c r="O15">
+        <f>6.65/2</f>
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="P15">
+        <f>6.62/2</f>
+        <v>3.31</v>
       </c>
       <c r="Q15" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.3133333333333339</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>7</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+      <c r="B16" s="19">
+        <v>5.57</v>
+      </c>
+      <c r="C16" s="19">
+        <v>5.86</v>
+      </c>
+      <c r="D16" s="19">
+        <v>5.64</v>
+      </c>
       <c r="E16" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.69</v>
+      </c>
+      <c r="F16" s="21">
+        <v>3.19</v>
+      </c>
+      <c r="G16" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="H16" s="21">
+        <v>3.23</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.206666666666667</v>
+      </c>
+      <c r="J16" s="21">
+        <v>11.99</v>
+      </c>
+      <c r="K16" s="21">
+        <v>10.84</v>
+      </c>
+      <c r="L16" s="21">
+        <v>11.47</v>
       </c>
       <c r="M16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.433333333333332</v>
+      </c>
+      <c r="N16" s="21">
+        <v>3.92</v>
+      </c>
+      <c r="O16" s="21">
+        <v>3.96</v>
+      </c>
+      <c r="P16" s="21">
+        <v>4.04</v>
       </c>
       <c r="Q16" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.9733333333333332</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
         <v>7.5</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="B17" s="19">
+        <v>6.36</v>
+      </c>
+      <c r="C17" s="19">
+        <v>6.37</v>
+      </c>
+      <c r="D17" s="19">
+        <v>6.11</v>
+      </c>
       <c r="E17" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.28</v>
+      </c>
+      <c r="F17" s="21">
+        <v>3.55</v>
+      </c>
+      <c r="G17" s="21">
+        <v>3.48</v>
+      </c>
+      <c r="H17" s="21">
+        <v>3.49</v>
       </c>
       <c r="I17" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5066666666666664</v>
+      </c>
+      <c r="J17" s="21">
+        <v>12.19</v>
+      </c>
+      <c r="K17" s="21">
+        <v>10.67</v>
+      </c>
+      <c r="L17" s="21">
+        <v>11.49</v>
       </c>
       <c r="M17" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.450000000000001</v>
+      </c>
+      <c r="N17" s="21">
+        <v>4.43</v>
+      </c>
+      <c r="O17" s="21">
+        <v>4.32</v>
+      </c>
+      <c r="P17" s="21">
+        <v>4.5599999999999996</v>
       </c>
       <c r="Q17" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.4366666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>